<commit_message>
Adding note about CBOR
</commit_message>
<xml_diff>
--- a/doc/IIX Code Charts.xlsx
+++ b/doc/IIX Code Charts.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13830" windowHeight="4920" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UTF-8" sheetId="3" r:id="rId1"/>
     <sheet name="IIX code categories" sheetId="2" r:id="rId2"/>
+    <sheet name="IIX code draft" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="UTF_8_code_chart">'UTF-8'!$A$1:$R$18</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
   <si>
     <t>_0</t>
   </si>
@@ -340,6 +341,57 @@
       </rPr>
       <t>IIX: Introducers</t>
     </r>
+  </si>
+  <si>
+    <t>1-byte values</t>
+  </si>
+  <si>
+    <t>1-byte types</t>
+  </si>
+  <si>
+    <t>variable-length values</t>
+  </si>
+  <si>
+    <t>variaable length types</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>UNK</t>
+  </si>
+  <si>
+    <t>NEG1</t>
+  </si>
+  <si>
+    <t>ZERO</t>
+  </si>
+  <si>
+    <t>POS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IIX Start-of-context = FF 00 </t>
+  </si>
+  <si>
+    <t>UTF-8 'BOM' = EF BB BF - not relevant or needed</t>
+  </si>
+  <si>
+    <t>1-byte types ?</t>
+  </si>
+  <si>
+    <t>SPS</t>
+  </si>
+  <si>
+    <t>Sep/term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPS - Special Seperator.   </t>
+  </si>
+  <si>
+    <t>POS2</t>
+  </si>
+  <si>
+    <t>NEG2</t>
   </si>
 </sst>
 </file>
@@ -516,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,6 +772,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="50">
     <border>
@@ -1389,7 +1447,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1440,9 +1498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="32" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1458,49 +1513,10 @@
     <xf numFmtId="0" fontId="17" fillId="33" borderId="11" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="26" xfId="39" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="26" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="39" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="39"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="28" xfId="39" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="29" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="33" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="17" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="23" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="34" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="35" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="37" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="28" xfId="31" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="39" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1510,9 +1526,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="41" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1549,26 +1562,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="29" xfId="31" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="24" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="49" xfId="34" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="36" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="32" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="35" borderId="31" xfId="22" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1595,23 +1590,98 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="25" xfId="40" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="23" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="17" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="22" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="21" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="26" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="26" xfId="39" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="25" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="25" xfId="40" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="23" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="36" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="17" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="32" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="22" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="21" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="24" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="29" xfId="31" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="28" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="37" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="35" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="34" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="23" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="17" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="33" xfId="31" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="29" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="28" xfId="39" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" xfId="34" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1970,859 +2040,859 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="4.77734375" style="11" customWidth="1"/>
-    <col min="18" max="18" width="19.77734375" style="21" customWidth="1"/>
-    <col min="19" max="19" width="25.6640625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="4.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="4.7109375" style="11" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" style="20" customWidth="1"/>
+    <col min="19" max="19" width="25.7109375" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-    </row>
-    <row r="2" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+    </row>
+    <row r="2" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="52" t="s">
+      <c r="O2" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="52" t="s">
+      <c r="P2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="51" t="s">
+      <c r="Q2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="58" t="s">
+      <c r="R2" s="40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+    <row r="3" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="M3" s="48" t="s">
+      <c r="M3" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="48" t="s">
+      <c r="O3" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="P3" s="48" t="s">
+      <c r="P3" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="Q3" s="47" t="s">
+      <c r="Q3" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="59" t="s">
+      <c r="R3" s="61" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:18" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="P4" s="45" t="s">
+      <c r="P4" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="Q4" s="39" t="s">
+      <c r="Q4" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="R4" s="42"/>
-    </row>
-    <row r="5" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="R4" s="62"/>
+    </row>
+    <row r="5" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="44" t="str">
+      <c r="B5" s="29" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C5" s="40" t="str">
-        <f>CHAR(CODE(B5)+1)</f>
+      <c r="C5" s="26" t="str">
+        <f t="shared" ref="C5:Q5" si="0">CHAR(CODE(B5)+1)</f>
         <v>!</v>
       </c>
-      <c r="D5" s="40" t="str">
-        <f>CHAR(CODE(C5)+1)</f>
+      <c r="D5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>"</v>
       </c>
-      <c r="E5" s="40" t="str">
-        <f>CHAR(CODE(D5)+1)</f>
+      <c r="E5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>#</v>
       </c>
-      <c r="F5" s="40" t="str">
-        <f>CHAR(CODE(E5)+1)</f>
+      <c r="F5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>$</v>
       </c>
-      <c r="G5" s="40" t="str">
-        <f>CHAR(CODE(F5)+1)</f>
+      <c r="G5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>%</v>
       </c>
-      <c r="H5" s="40" t="str">
-        <f>CHAR(CODE(G5)+1)</f>
+      <c r="H5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>&amp;</v>
       </c>
-      <c r="I5" s="40" t="str">
-        <f>CHAR(CODE(H5)+1)</f>
+      <c r="I5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>'</v>
       </c>
-      <c r="J5" s="40" t="str">
-        <f>CHAR(CODE(I5)+1)</f>
+      <c r="J5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>(</v>
       </c>
-      <c r="K5" s="40" t="str">
-        <f>CHAR(CODE(J5)+1)</f>
+      <c r="K5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>)</v>
       </c>
-      <c r="L5" s="40" t="str">
-        <f>CHAR(CODE(K5)+1)</f>
+      <c r="L5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>*</v>
       </c>
-      <c r="M5" s="40" t="str">
-        <f>CHAR(CODE(L5)+1)</f>
+      <c r="M5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="N5" s="40" t="str">
-        <f>CHAR(CODE(M5)+1)</f>
+      <c r="N5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
-      <c r="O5" s="40" t="str">
-        <f>CHAR(CODE(N5)+1)</f>
+      <c r="O5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="P5" s="40" t="str">
-        <f>CHAR(CODE(O5)+1)</f>
+      <c r="P5" s="26" t="str">
+        <f t="shared" si="0"/>
         <v>.</v>
       </c>
-      <c r="Q5" s="43" t="str">
-        <f>CHAR(CODE(P5)+1)</f>
+      <c r="Q5" s="28" t="str">
+        <f t="shared" si="0"/>
         <v>/</v>
       </c>
-      <c r="R5" s="42"/>
-    </row>
-    <row r="6" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="R5" s="62"/>
+    </row>
+    <row r="6" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="41" t="str">
+      <c r="B6" s="27" t="str">
         <f>CHAR(CODE(Q5)+1)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="40" t="str">
-        <f>CHAR(CODE(B6)+1)</f>
+      <c r="C6" s="26" t="str">
+        <f t="shared" ref="C6:Q6" si="1">CHAR(CODE(B6)+1)</f>
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="str">
-        <f>CHAR(CODE(C6)+1)</f>
+      <c r="D6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E6" s="40" t="str">
-        <f>CHAR(CODE(D6)+1)</f>
+      <c r="E6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F6" s="40" t="str">
-        <f>CHAR(CODE(E6)+1)</f>
+      <c r="F6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G6" s="40" t="str">
-        <f>CHAR(CODE(F6)+1)</f>
+      <c r="G6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H6" s="40" t="str">
-        <f>CHAR(CODE(G6)+1)</f>
+      <c r="H6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I6" s="40" t="str">
-        <f>CHAR(CODE(H6)+1)</f>
+      <c r="I6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J6" s="40" t="str">
-        <f>CHAR(CODE(I6)+1)</f>
+      <c r="J6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K6" s="40" t="str">
-        <f>CHAR(CODE(J6)+1)</f>
+      <c r="K6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L6" s="40" t="str">
-        <f>CHAR(CODE(K6)+1)</f>
+      <c r="L6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>:</v>
       </c>
-      <c r="M6" s="40" t="str">
-        <f>CHAR(CODE(L6)+1)</f>
+      <c r="M6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>;</v>
       </c>
-      <c r="N6" s="40" t="str">
-        <f>CHAR(CODE(M6)+1)</f>
+      <c r="N6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>&lt;</v>
       </c>
-      <c r="O6" s="40" t="str">
-        <f>CHAR(CODE(N6)+1)</f>
+      <c r="O6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>=</v>
       </c>
-      <c r="P6" s="40" t="str">
-        <f>CHAR(CODE(O6)+1)</f>
+      <c r="P6" s="26" t="str">
+        <f t="shared" si="1"/>
         <v>&gt;</v>
       </c>
-      <c r="Q6" s="43" t="str">
-        <f>CHAR(CODE(P6)+1)</f>
+      <c r="Q6" s="28" t="str">
+        <f t="shared" si="1"/>
         <v>?</v>
       </c>
-      <c r="R6" s="42"/>
-    </row>
-    <row r="7" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="R6" s="62"/>
+    </row>
+    <row r="7" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="41" t="str">
+      <c r="B7" s="27" t="str">
         <f>CHAR(CODE(Q6)+1)</f>
         <v>@</v>
       </c>
-      <c r="C7" s="40" t="str">
-        <f>CHAR(CODE(B7)+1)</f>
+      <c r="C7" s="26" t="str">
+        <f t="shared" ref="C7:Q7" si="2">CHAR(CODE(B7)+1)</f>
         <v>A</v>
       </c>
-      <c r="D7" s="40" t="str">
-        <f>CHAR(CODE(C7)+1)</f>
+      <c r="D7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>B</v>
       </c>
-      <c r="E7" s="40" t="str">
-        <f>CHAR(CODE(D7)+1)</f>
+      <c r="E7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>C</v>
       </c>
-      <c r="F7" s="40" t="str">
-        <f>CHAR(CODE(E7)+1)</f>
+      <c r="F7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>D</v>
       </c>
-      <c r="G7" s="40" t="str">
-        <f>CHAR(CODE(F7)+1)</f>
+      <c r="G7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>E</v>
       </c>
-      <c r="H7" s="40" t="str">
-        <f>CHAR(CODE(G7)+1)</f>
+      <c r="H7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="I7" s="40" t="str">
-        <f>CHAR(CODE(H7)+1)</f>
+      <c r="I7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>G</v>
       </c>
-      <c r="J7" s="40" t="str">
-        <f>CHAR(CODE(I7)+1)</f>
+      <c r="J7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>H</v>
       </c>
-      <c r="K7" s="40" t="str">
-        <f>CHAR(CODE(J7)+1)</f>
+      <c r="K7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>I</v>
       </c>
-      <c r="L7" s="40" t="str">
-        <f>CHAR(CODE(K7)+1)</f>
+      <c r="L7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>J</v>
       </c>
-      <c r="M7" s="40" t="str">
-        <f>CHAR(CODE(L7)+1)</f>
+      <c r="M7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>K</v>
       </c>
-      <c r="N7" s="40" t="str">
-        <f>CHAR(CODE(M7)+1)</f>
+      <c r="N7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>L</v>
       </c>
-      <c r="O7" s="40" t="str">
-        <f>CHAR(CODE(N7)+1)</f>
+      <c r="O7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>M</v>
       </c>
-      <c r="P7" s="40" t="str">
-        <f>CHAR(CODE(O7)+1)</f>
+      <c r="P7" s="26" t="str">
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
-      <c r="Q7" s="43" t="str">
-        <f>CHAR(CODE(P7)+1)</f>
+      <c r="Q7" s="28" t="str">
+        <f t="shared" si="2"/>
         <v>O</v>
       </c>
-      <c r="R7" s="42"/>
-    </row>
-    <row r="8" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="R7" s="62"/>
+    </row>
+    <row r="8" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="41" t="str">
+      <c r="B8" s="27" t="str">
         <f>CHAR(CODE(Q7)+1)</f>
         <v>P</v>
       </c>
-      <c r="C8" s="40" t="str">
-        <f>CHAR(CODE(B8)+1)</f>
+      <c r="C8" s="26" t="str">
+        <f t="shared" ref="C8:Q8" si="3">CHAR(CODE(B8)+1)</f>
         <v>Q</v>
       </c>
-      <c r="D8" s="40" t="str">
-        <f>CHAR(CODE(C8)+1)</f>
+      <c r="D8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>R</v>
       </c>
-      <c r="E8" s="40" t="str">
-        <f>CHAR(CODE(D8)+1)</f>
+      <c r="E8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="F8" s="40" t="str">
-        <f>CHAR(CODE(E8)+1)</f>
+      <c r="F8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>T</v>
       </c>
-      <c r="G8" s="40" t="str">
-        <f>CHAR(CODE(F8)+1)</f>
+      <c r="G8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>U</v>
       </c>
-      <c r="H8" s="40" t="str">
-        <f>CHAR(CODE(G8)+1)</f>
+      <c r="H8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>V</v>
       </c>
-      <c r="I8" s="40" t="str">
-        <f>CHAR(CODE(H8)+1)</f>
+      <c r="I8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>W</v>
       </c>
-      <c r="J8" s="40" t="str">
-        <f>CHAR(CODE(I8)+1)</f>
+      <c r="J8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="K8" s="40" t="str">
-        <f>CHAR(CODE(J8)+1)</f>
+      <c r="K8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>Y</v>
       </c>
-      <c r="L8" s="40" t="str">
-        <f>CHAR(CODE(K8)+1)</f>
+      <c r="L8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>Z</v>
       </c>
-      <c r="M8" s="40" t="str">
-        <f>CHAR(CODE(L8)+1)</f>
+      <c r="M8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>[</v>
       </c>
-      <c r="N8" s="40" t="str">
-        <f>CHAR(CODE(M8)+1)</f>
+      <c r="N8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>\</v>
       </c>
-      <c r="O8" s="40" t="str">
-        <f>CHAR(CODE(N8)+1)</f>
+      <c r="O8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>]</v>
       </c>
-      <c r="P8" s="40" t="str">
-        <f>CHAR(CODE(O8)+1)</f>
+      <c r="P8" s="26" t="str">
+        <f t="shared" si="3"/>
         <v>^</v>
       </c>
-      <c r="Q8" s="43" t="str">
-        <f>CHAR(CODE(P8)+1)</f>
+      <c r="Q8" s="28" t="str">
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
-      <c r="R8" s="42"/>
-    </row>
-    <row r="9" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="R8" s="62"/>
+    </row>
+    <row r="9" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="41" t="str">
+      <c r="B9" s="27" t="str">
         <f>CHAR(CODE(Q8)+1)</f>
         <v>`</v>
       </c>
-      <c r="C9" s="40" t="str">
-        <f>CHAR(CODE(B9)+1)</f>
+      <c r="C9" s="26" t="str">
+        <f t="shared" ref="C9:Q9" si="4">CHAR(CODE(B9)+1)</f>
         <v>a</v>
       </c>
-      <c r="D9" s="40" t="str">
-        <f>CHAR(CODE(C9)+1)</f>
+      <c r="D9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>b</v>
       </c>
-      <c r="E9" s="40" t="str">
-        <f>CHAR(CODE(D9)+1)</f>
+      <c r="E9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>c</v>
       </c>
-      <c r="F9" s="40" t="str">
-        <f>CHAR(CODE(E9)+1)</f>
+      <c r="F9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>d</v>
       </c>
-      <c r="G9" s="40" t="str">
-        <f>CHAR(CODE(F9)+1)</f>
+      <c r="G9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>e</v>
       </c>
-      <c r="H9" s="40" t="str">
-        <f>CHAR(CODE(G9)+1)</f>
+      <c r="H9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>f</v>
       </c>
-      <c r="I9" s="40" t="str">
-        <f>CHAR(CODE(H9)+1)</f>
+      <c r="I9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>g</v>
       </c>
-      <c r="J9" s="40" t="str">
-        <f>CHAR(CODE(I9)+1)</f>
+      <c r="J9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>h</v>
       </c>
-      <c r="K9" s="40" t="str">
-        <f>CHAR(CODE(J9)+1)</f>
+      <c r="K9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>i</v>
       </c>
-      <c r="L9" s="40" t="str">
-        <f>CHAR(CODE(K9)+1)</f>
+      <c r="L9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>j</v>
       </c>
-      <c r="M9" s="40" t="str">
-        <f>CHAR(CODE(L9)+1)</f>
+      <c r="M9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>k</v>
       </c>
-      <c r="N9" s="40" t="str">
-        <f>CHAR(CODE(M9)+1)</f>
+      <c r="N9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>l</v>
       </c>
-      <c r="O9" s="40" t="str">
-        <f>CHAR(CODE(N9)+1)</f>
+      <c r="O9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>m</v>
       </c>
-      <c r="P9" s="40" t="str">
-        <f>CHAR(CODE(O9)+1)</f>
+      <c r="P9" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>n</v>
       </c>
-      <c r="Q9" s="43" t="str">
-        <f>CHAR(CODE(P9)+1)</f>
+      <c r="Q9" s="28" t="str">
+        <f t="shared" si="4"/>
         <v>o</v>
       </c>
-      <c r="R9" s="42"/>
-    </row>
-    <row r="10" spans="1:18" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="R9" s="62"/>
+    </row>
+    <row r="10" spans="1:18" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41" t="str">
+      <c r="B10" s="27" t="str">
         <f>CHAR(CODE(Q9)+1)</f>
         <v>p</v>
       </c>
-      <c r="C10" s="40" t="str">
-        <f>CHAR(CODE(B10)+1)</f>
+      <c r="C10" s="26" t="str">
+        <f t="shared" ref="C10:P10" si="5">CHAR(CODE(B10)+1)</f>
         <v>q</v>
       </c>
-      <c r="D10" s="40" t="str">
-        <f>CHAR(CODE(C10)+1)</f>
+      <c r="D10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>r</v>
       </c>
-      <c r="E10" s="40" t="str">
-        <f>CHAR(CODE(D10)+1)</f>
+      <c r="E10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>s</v>
       </c>
-      <c r="F10" s="40" t="str">
-        <f>CHAR(CODE(E10)+1)</f>
+      <c r="F10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>t</v>
       </c>
-      <c r="G10" s="40" t="str">
-        <f>CHAR(CODE(F10)+1)</f>
+      <c r="G10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>u</v>
       </c>
-      <c r="H10" s="40" t="str">
-        <f>CHAR(CODE(G10)+1)</f>
+      <c r="H10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>v</v>
       </c>
-      <c r="I10" s="40" t="str">
-        <f>CHAR(CODE(H10)+1)</f>
+      <c r="I10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>w</v>
       </c>
-      <c r="J10" s="40" t="str">
-        <f>CHAR(CODE(I10)+1)</f>
+      <c r="J10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>x</v>
       </c>
-      <c r="K10" s="40" t="str">
-        <f>CHAR(CODE(J10)+1)</f>
+      <c r="K10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>y</v>
       </c>
-      <c r="L10" s="40" t="str">
-        <f>CHAR(CODE(K10)+1)</f>
+      <c r="L10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>z</v>
       </c>
-      <c r="M10" s="40" t="str">
-        <f>CHAR(CODE(L10)+1)</f>
+      <c r="M10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>{</v>
       </c>
-      <c r="N10" s="40" t="str">
-        <f>CHAR(CODE(M10)+1)</f>
+      <c r="N10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>|</v>
       </c>
-      <c r="O10" s="40" t="str">
-        <f>CHAR(CODE(N10)+1)</f>
+      <c r="O10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>}</v>
       </c>
-      <c r="P10" s="40" t="str">
-        <f>CHAR(CODE(O10)+1)</f>
+      <c r="P10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>~</v>
       </c>
-      <c r="Q10" s="39" t="s">
+      <c r="Q10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="38"/>
-    </row>
-    <row r="11" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="R10" s="63"/>
+    </row>
+    <row r="11" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="60" t="s">
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="59" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="61"/>
-    </row>
-    <row r="13" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="B12" s="68"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="70"/>
+      <c r="R12" s="60"/>
+    </row>
+    <row r="13" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="61"/>
-    </row>
-    <row r="14" spans="1:18" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="60"/>
+    </row>
+    <row r="14" spans="1:18" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="61"/>
-    </row>
-    <row r="15" spans="1:18" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+      <c r="B14" s="71"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
+      <c r="O14" s="72"/>
+      <c r="P14" s="72"/>
+      <c r="Q14" s="73"/>
+      <c r="R14" s="60"/>
+    </row>
+    <row r="15" spans="1:18" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="62" t="str">
+      <c r="B15" s="41" t="str">
         <f>"C0"</f>
         <v>C0</v>
       </c>
-      <c r="C15" s="63" t="str">
+      <c r="C15" s="42" t="str">
         <f>DEC2HEX(HEX2DEC(B15)+1,2)</f>
         <v>C1</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="64" t="s">
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="43" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="25" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="57" t="s">
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="64" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="71" t="s">
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="72"/>
-      <c r="R17" s="57"/>
-    </row>
-    <row r="18" spans="1:18" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="64"/>
+    </row>
+    <row r="18" spans="1:18" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="74"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="65" t="s">
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(G18)+1,2)</f>
+      <c r="H18" s="45" t="str">
+        <f t="shared" ref="H18:Q18" si="6">DEC2HEX(HEX2DEC(G18)+1,2)</f>
         <v>F6</v>
       </c>
-      <c r="I18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(H18)+1,2)</f>
+      <c r="I18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>F7</v>
       </c>
-      <c r="J18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(I18)+1,2)</f>
+      <c r="J18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>F8</v>
       </c>
-      <c r="K18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(J18)+1,2)</f>
+      <c r="K18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>F9</v>
       </c>
-      <c r="L18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(K18)+1,2)</f>
+      <c r="L18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>FA</v>
       </c>
-      <c r="M18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(L18)+1,2)</f>
+      <c r="M18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>FB</v>
       </c>
-      <c r="N18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(M18)+1,2)</f>
+      <c r="N18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>FC</v>
       </c>
-      <c r="O18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(N18)+1,2)</f>
+      <c r="O18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>FD</v>
       </c>
-      <c r="P18" s="66" t="str">
-        <f>DEC2HEX(HEX2DEC(O18)+1,2)</f>
+      <c r="P18" s="45" t="str">
+        <f t="shared" si="6"/>
         <v>FE</v>
       </c>
-      <c r="Q18" s="67" t="str">
-        <f>DEC2HEX(HEX2DEC(P18)+1,2)</f>
+      <c r="Q18" s="46" t="str">
+        <f t="shared" si="6"/>
         <v>FF</v>
       </c>
-      <c r="R18" s="68" t="s">
+      <c r="R18" s="47" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -2840,7 +2910,7 @@
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -2858,7 +2928,7 @@
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -2876,7 +2946,7 @@
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2894,7 +2964,7 @@
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -2912,7 +2982,7 @@
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -2930,7 +3000,7 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -2948,7 +3018,7 @@
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -2966,7 +3036,7 @@
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -2984,7 +3054,7 @@
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -3002,7 +3072,7 @@
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -3020,7 +3090,7 @@
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -3038,7 +3108,7 @@
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -3056,7 +3126,7 @@
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -3074,7 +3144,7 @@
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -3092,7 +3162,7 @@
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -3132,40 +3202,40 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
-    <col min="2" max="17" width="3.77734375" style="11" customWidth="1"/>
-    <col min="18" max="18" width="1.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="17" width="3.7109375" style="11" customWidth="1"/>
+    <col min="18" max="18" width="1.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="14" style="2" customWidth="1"/>
-    <col min="20" max="20" width="15" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="1"/>
+    <col min="20" max="20" width="23.85546875" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="12" t="s">
         <v>0</v>
@@ -3223,7 +3293,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -3299,7 +3369,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -3375,7 +3445,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -3451,7 +3521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -3527,7 +3597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -3603,7 +3673,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -3679,7 +3749,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -3755,7 +3825,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -3831,70 +3901,70 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="18">
         <v>40</v>
       </c>
-      <c r="C11" s="19" t="str">
+      <c r="C11" s="18" t="str">
         <f>DEC2HEX(HEX2DEC(B11)+1,2)</f>
         <v>41</v>
       </c>
-      <c r="D11" s="19" t="str">
+      <c r="D11" s="18" t="str">
         <f t="shared" ref="D11:Q11" si="18">DEC2HEX(HEX2DEC(C11)+1,2)</f>
         <v>42</v>
       </c>
-      <c r="E11" s="19" t="str">
+      <c r="E11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>43</v>
       </c>
-      <c r="F11" s="19" t="str">
+      <c r="F11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>44</v>
       </c>
-      <c r="G11" s="19" t="str">
+      <c r="G11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>45</v>
       </c>
-      <c r="H11" s="19" t="str">
+      <c r="H11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>46</v>
       </c>
-      <c r="I11" s="19" t="str">
+      <c r="I11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>47</v>
       </c>
-      <c r="J11" s="19" t="str">
+      <c r="J11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>48</v>
       </c>
-      <c r="K11" s="19" t="str">
+      <c r="K11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>49</v>
       </c>
-      <c r="L11" s="19" t="str">
+      <c r="L11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>4A</v>
       </c>
-      <c r="M11" s="19" t="str">
+      <c r="M11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>4B</v>
       </c>
-      <c r="N11" s="19" t="str">
+      <c r="N11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>4C</v>
       </c>
-      <c r="O11" s="19" t="str">
+      <c r="O11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>4D</v>
       </c>
-      <c r="P11" s="19" t="str">
+      <c r="P11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>4E</v>
       </c>
-      <c r="Q11" s="19" t="str">
+      <c r="Q11" s="18" t="str">
         <f t="shared" si="18"/>
         <v>4F</v>
       </c>
@@ -3902,73 +3972,75 @@
       <c r="S11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="T11"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="19" t="str">
+      <c r="B12" s="18" t="str">
         <f>DEC2HEX(HEX2DEC(Q11)+1,2)</f>
         <v>50</v>
       </c>
-      <c r="C12" s="19" t="str">
+      <c r="C12" s="18" t="str">
         <f>DEC2HEX(HEX2DEC(B12)+1,2)</f>
         <v>51</v>
       </c>
-      <c r="D12" s="19" t="str">
+      <c r="D12" s="18" t="str">
         <f t="shared" ref="D12:Q14" si="19">DEC2HEX(HEX2DEC(C12)+1,2)</f>
         <v>52</v>
       </c>
-      <c r="E12" s="19" t="str">
+      <c r="E12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>53</v>
       </c>
-      <c r="F12" s="19" t="str">
+      <c r="F12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>54</v>
       </c>
-      <c r="G12" s="19" t="str">
+      <c r="G12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>55</v>
       </c>
-      <c r="H12" s="19" t="str">
+      <c r="H12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>56</v>
       </c>
-      <c r="I12" s="19" t="str">
+      <c r="I12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>57</v>
       </c>
-      <c r="J12" s="19" t="str">
+      <c r="J12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>58</v>
       </c>
-      <c r="K12" s="19" t="str">
+      <c r="K12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>59</v>
       </c>
-      <c r="L12" s="19" t="str">
+      <c r="L12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>5A</v>
       </c>
-      <c r="M12" s="19" t="str">
+      <c r="M12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>5B</v>
       </c>
-      <c r="N12" s="19" t="str">
+      <c r="N12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>5C</v>
       </c>
-      <c r="O12" s="19" t="str">
+      <c r="O12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>5D</v>
       </c>
-      <c r="P12" s="19" t="str">
+      <c r="P12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>5E</v>
       </c>
-      <c r="Q12" s="19" t="str">
+      <c r="Q12" s="18" t="str">
         <f t="shared" si="19"/>
         <v>5F</v>
       </c>
@@ -3976,73 +4048,75 @@
       <c r="S12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="T12"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="19" t="str">
+      <c r="B13" s="18" t="str">
         <f>DEC2HEX(HEX2DEC(Q12)+1,2)</f>
         <v>60</v>
       </c>
-      <c r="C13" s="19" t="str">
+      <c r="C13" s="18" t="str">
         <f>DEC2HEX(HEX2DEC(B13)+1,2)</f>
         <v>61</v>
       </c>
-      <c r="D13" s="19" t="str">
+      <c r="D13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>62</v>
       </c>
-      <c r="E13" s="19" t="str">
+      <c r="E13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>63</v>
       </c>
-      <c r="F13" s="19" t="str">
+      <c r="F13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>64</v>
       </c>
-      <c r="G13" s="19" t="str">
+      <c r="G13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>65</v>
       </c>
-      <c r="H13" s="19" t="str">
+      <c r="H13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>66</v>
       </c>
-      <c r="I13" s="19" t="str">
+      <c r="I13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
-      <c r="J13" s="19" t="str">
+      <c r="J13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>68</v>
       </c>
-      <c r="K13" s="19" t="str">
+      <c r="K13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>69</v>
       </c>
-      <c r="L13" s="19" t="str">
+      <c r="L13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>6A</v>
       </c>
-      <c r="M13" s="19" t="str">
+      <c r="M13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>6B</v>
       </c>
-      <c r="N13" s="19" t="str">
+      <c r="N13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>6C</v>
       </c>
-      <c r="O13" s="19" t="str">
+      <c r="O13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>6D</v>
       </c>
-      <c r="P13" s="19" t="str">
+      <c r="P13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>6E</v>
       </c>
-      <c r="Q13" s="19" t="str">
+      <c r="Q13" s="18" t="str">
         <f t="shared" si="19"/>
         <v>6F</v>
       </c>
@@ -4050,73 +4124,75 @@
       <c r="S13" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="T13"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="19" t="str">
+      <c r="B14" s="18" t="str">
         <f>DEC2HEX(HEX2DEC(Q13)+1,2)</f>
         <v>70</v>
       </c>
-      <c r="C14" s="19" t="str">
+      <c r="C14" s="18" t="str">
         <f>DEC2HEX(HEX2DEC(B14)+1,2)</f>
         <v>71</v>
       </c>
-      <c r="D14" s="19" t="str">
+      <c r="D14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>72</v>
       </c>
-      <c r="E14" s="19" t="str">
+      <c r="E14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>73</v>
       </c>
-      <c r="F14" s="19" t="str">
+      <c r="F14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>74</v>
       </c>
-      <c r="G14" s="19" t="str">
+      <c r="G14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>75</v>
       </c>
-      <c r="H14" s="19" t="str">
+      <c r="H14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>76</v>
       </c>
-      <c r="I14" s="19" t="str">
+      <c r="I14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>77</v>
       </c>
-      <c r="J14" s="19" t="str">
+      <c r="J14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>78</v>
       </c>
-      <c r="K14" s="19" t="str">
+      <c r="K14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>79</v>
       </c>
-      <c r="L14" s="19" t="str">
+      <c r="L14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>7A</v>
       </c>
-      <c r="M14" s="19" t="str">
+      <c r="M14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>7B</v>
       </c>
-      <c r="N14" s="19" t="str">
+      <c r="N14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>7C</v>
       </c>
-      <c r="O14" s="19" t="str">
+      <c r="O14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>7D</v>
       </c>
-      <c r="P14" s="19" t="str">
+      <c r="P14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>7E</v>
       </c>
-      <c r="Q14" s="19" t="str">
+      <c r="Q14" s="18" t="str">
         <f t="shared" si="19"/>
         <v>7F</v>
       </c>
@@ -4124,9 +4200,11 @@
       <c r="S14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="T14"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -4136,58 +4214,58 @@
       <c r="C15" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>12</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <f>D15</f>
         <v>12</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <f t="shared" ref="F15:Q15" si="20">E15</f>
         <v>12</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="P15" s="20">
+      <c r="P15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
-      <c r="Q15" s="20">
+      <c r="Q15" s="19">
         <f t="shared" si="20"/>
         <v>12</v>
       </c>
@@ -4199,71 +4277,71 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="19">
         <f>Q15</f>
         <v>12</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="19">
         <f>B16</f>
         <v>12</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="19">
         <f t="shared" ref="D16:Q17" si="21">C16</f>
         <v>12</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="L16" s="20">
+      <c r="L16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="M16" s="20">
+      <c r="M16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="N16" s="20">
+      <c r="N16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="O16" s="20">
+      <c r="O16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="P16" s="20">
+      <c r="P16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
-      <c r="Q16" s="20">
+      <c r="Q16" s="19">
         <f t="shared" si="21"/>
         <v>12</v>
       </c>
@@ -4273,70 +4351,70 @@
       </c>
       <c r="T16"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <v>13</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <f>B17</f>
         <v>13</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="L17" s="20">
+      <c r="L17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="M17" s="20">
+      <c r="M17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="N17" s="20">
+      <c r="N17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="O17" s="20">
+      <c r="O17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="P17" s="20">
+      <c r="P17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
-      <c r="Q17" s="20">
+      <c r="Q17" s="19">
         <f t="shared" si="21"/>
         <v>13</v>
       </c>
@@ -4346,26 +4424,26 @@
       </c>
       <c r="T17"/>
     </row>
-    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <v>14</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <f>B18</f>
         <v>14</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="19">
         <f>C18</f>
         <v>14</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="19">
         <f>D18</f>
         <v>14</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <f>E18</f>
         <v>14</v>
       </c>
@@ -4410,10 +4488,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -4431,7 +4509,7 @@
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -4449,7 +4527,7 @@
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4467,7 +4545,7 @@
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -4485,7 +4563,7 @@
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -4503,7 +4581,7 @@
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -4521,7 +4599,7 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -4539,7 +4617,7 @@
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -4557,7 +4635,7 @@
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -4575,7 +4653,7 @@
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -4593,7 +4671,7 @@
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -4611,7 +4689,7 @@
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -4629,7 +4707,7 @@
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -4647,7 +4725,7 @@
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -4665,7 +4743,7 @@
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -4683,7 +4761,7 @@
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -4708,4 +4786,836 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="17" width="7.85546875" style="11" customWidth="1"/>
+    <col min="18" max="18" width="1.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.85546875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2"/>
+      <c r="S2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3"/>
+      <c r="S3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4"/>
+      <c r="S4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5"/>
+      <c r="S5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
+      <c r="R6"/>
+      <c r="S6"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
+      <c r="R7"/>
+      <c r="S7"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8"/>
+      <c r="S8"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
+      <c r="Q9" s="77"/>
+      <c r="R9"/>
+      <c r="S9"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="77"/>
+      <c r="Q10" s="77"/>
+      <c r="R10"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="79" t="s">
+        <v>116</v>
+      </c>
+      <c r="N11" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="O11" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="P11" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="R11"/>
+      <c r="S11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="79"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12"/>
+      <c r="S12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13"/>
+      <c r="S13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14"/>
+      <c r="S14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="78"/>
+      <c r="N15" s="78"/>
+      <c r="O15" s="78"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78"/>
+      <c r="R15"/>
+      <c r="S15"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="78"/>
+      <c r="N16" s="78"/>
+      <c r="O16" s="78"/>
+      <c r="P16" s="78"/>
+      <c r="Q16" s="78"/>
+      <c r="R16"/>
+      <c r="S16"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
+      <c r="L17" s="78"/>
+      <c r="M17" s="78"/>
+      <c r="N17" s="78"/>
+      <c r="O17" s="78"/>
+      <c r="P17" s="78"/>
+      <c r="Q17" s="78"/>
+      <c r="R17"/>
+      <c r="S17"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q18" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="R18"/>
+      <c r="S18"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+    </row>
+    <row r="21" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="80"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="M21" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="A21:F21"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>